<commit_message>
Avances del 18 de julio
</commit_message>
<xml_diff>
--- a/Umbrales.xlsx
+++ b/Umbrales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisc\OneDrive\Documentos\GitHub\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{8CA12F8F-B3D8-4C6C-A0EB-BD07F2DF7665}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{E3B24207-D8D3-4B6C-9B18-C64F7B15665C}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{8CA12F8F-B3D8-4C6C-A0EB-BD07F2DF7665}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{F1129FDB-6861-43DD-A9FF-F9552BFA4D4E}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{245771D3-793C-48D1-9BFB-02CA341459F9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>device_name</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Compresor de Aire 3 60 HP</t>
   </si>
   <si>
-    <t>Compresor de Aire 4 60 HP</t>
-  </si>
-  <si>
     <t>Compresor de Amoniaco 1 Tornillo 250 HP</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
   </si>
   <si>
     <t>CAIR3</t>
-  </si>
-  <si>
-    <t>CAIR4</t>
   </si>
   <si>
     <t>CRT1</t>
@@ -505,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE91961D-1429-4ACA-BE3F-80C3668F3EDF}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,10 +515,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -532,10 +526,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>33.835000000000008</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -543,10 +537,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>27.953062500000001</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -554,10 +548,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>10.748747741935485</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -565,10 +559,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -576,10 +570,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>10.433578064516132</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -587,10 +581,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>34.353616774193547</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -598,10 +592,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>25.625</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -609,10 +603,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>28.765301935483873</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -620,10 +614,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>32.991250000000001</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -631,10 +625,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>27.081500000000002</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -642,10 +636,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>27.152407096774198</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -653,43 +647,43 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>33.140562500000001</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>13.531125000000001</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>13.518750000000001</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>180</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -697,10 +691,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>180</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -708,10 +702,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -722,18 +716,7 @@
         <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>77</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>